<commit_message>
Modifs mineures (05/04/21) 2
</commit_message>
<xml_diff>
--- a/data/template_portfolio_v2.xlsx
+++ b/data/template_portfolio_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALEXIS\PycharmProjects\Crypto_portfolio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0F6002-2C40-4031-8BD4-92E5F2A73792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89962E7C-DCBD-4DEA-B2BE-39FEB9D555C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="5" r:id="rId1"/>
@@ -20,8 +20,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cours_Cryptos!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Historique_Cryptos!$A$2:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Historique_Cryptos!$A$2:$Q$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Historique_EUR!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -53,21 +54,6 @@
     <t>Coin</t>
   </si>
   <si>
-    <t>ADA</t>
-  </si>
-  <si>
-    <t>CRYPTO</t>
-  </si>
-  <si>
-    <t>Quantité possédée</t>
-  </si>
-  <si>
-    <t>Date dernière transaction</t>
-  </si>
-  <si>
-    <t>Date première transaction</t>
-  </si>
-  <si>
     <t>Evolution prix sur 24h (en %)</t>
   </si>
   <si>
@@ -95,30 +81,6 @@
     <t>Prix total (en $)</t>
   </si>
   <si>
-    <t>Prix moyen vente</t>
-  </si>
-  <si>
-    <t>Prix moyen achat</t>
-  </si>
-  <si>
-    <t>Investissement</t>
-  </si>
-  <si>
-    <t>Valeur actuelle ($)</t>
-  </si>
-  <si>
-    <t>Gain/Perte ($)</t>
-  </si>
-  <si>
-    <t>ROI (%)</t>
-  </si>
-  <si>
-    <t>Variation 24h (%)</t>
-  </si>
-  <si>
-    <t>Prix actuel ($)</t>
-  </si>
-  <si>
     <t>Prix moyen d'achat (cumulé)</t>
   </si>
   <si>
@@ -150,6 +112,15 @@
   </si>
   <si>
     <t>VISION DETAILLEE</t>
+  </si>
+  <si>
+    <t>Solde de tokens</t>
+  </si>
+  <si>
+    <t>Quantité achetée (cumulée en $)</t>
+  </si>
+  <si>
+    <t>Quantité vendue (cumulée en $)</t>
   </si>
 </sst>
 </file>
@@ -162,8 +133,8 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0.00000_ ;_-[$$-409]* \-#,##0.00000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00000_ ;_-[$$-409]* \-#,##0.00000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -274,25 +245,24 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -302,13 +272,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -624,84 +594,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C446407-6BAA-4CE0-9012-7C420B72389B}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="3" customWidth="1"/>
+    <col min="6" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="9" max="9" width="37.28515625" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" style="3" customWidth="1"/>
+    <col min="11" max="12" width="21.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="A1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="L1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="H2">
-        <f>B2*L2</f>
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <f>H2-G2</f>
-        <v>0</v>
-      </c>
-      <c r="J2" t="e">
-        <f>I2/G2</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L1" xr:uid="{62EEAA3C-C037-4C96-99D3-CBEF41A29DD3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -711,31 +665,31 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="20.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="5"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>11</v>
+      <c r="E1" s="11" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -748,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,8 +715,8 @@
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -773,26 +727,26 @@
     <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
       <c r="J1" s="17" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="K1" s="17"/>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="18" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
@@ -809,46 +763,46 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="M2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>33</v>
+      <c r="N2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1029,7 +983,7 @@
       <c r="I39"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I2" xr:uid="{54136DF3-DFEF-41B2-B155-667CF4F80A02}"/>
+  <autoFilter ref="A2:Q2" xr:uid="{5C015313-19DF-4A4D-95DF-92A055C84E20}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="J1:M1"/>
@@ -1044,25 +998,25 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>13</v>
+      <c r="B1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>